<commit_message>
last push of this branch, new branch using new lib wil be uploaded
</commit_message>
<xml_diff>
--- a/Lasergun received.xlsx
+++ b/Lasergun received.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myrdd\Documents\2021-2022\di\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myrdd\Documents\PlatformIO\Projects\electronics test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F47C0038-0FC7-4275-8BC8-0ED781AF3657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987732C4-EB8B-417B-8B52-2DE4D1C760FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1200" yWindow="2205" windowWidth="21585" windowHeight="10965" xr2:uid="{F5CC861B-AF5E-4288-8C80-814FB9371A0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5CC861B-AF5E-4288-8C80-814FB9371A0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -446,10 +446,13 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>